<commit_message>
Contactpage changes with dynamic Radiobutton
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/Testdata.xlsx
+++ b/src/main/java/com/crm/qa/testdata/Testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Contacts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:K6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>Uname</t>
   </si>
@@ -87,13 +88,19 @@
     <t>callstatus</t>
   </si>
   <si>
-    <t>Shloka</t>
-  </si>
-  <si>
-    <t>pra</t>
-  </si>
-  <si>
-    <t>shloka@gmail.com</t>
+    <t>textstatus</t>
+  </si>
+  <si>
+    <t>emailstatus</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Nickc@gmail.com</t>
   </si>
   <si>
     <t>22056 barrington way</t>
@@ -114,10 +121,16 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Mahika</t>
-  </si>
-  <si>
-    <t>Mahika@gmail.com</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>cook</t>
+  </si>
+  <si>
+    <t>Nickolascook@gmail.com</t>
   </si>
   <si>
     <t>22026 barrington way</t>
@@ -127,9 +140,6 @@
   </si>
   <si>
     <t>Customer</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Shlok</t>
@@ -195,9 +205,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -209,15 +219,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,6 +252,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -253,14 +279,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -272,6 +290,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -279,32 +321,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,6 +336,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -327,37 +352,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,25 +394,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,55 +538,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,91 +568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,6 +600,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -608,23 +657,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -655,30 +689,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -690,155 +700,155 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1215,7 +1225,7 @@
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -1300,22 +1310,23 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="5"/>
   <cols>
-    <col min="3" max="3" width="22.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="28.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="22.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="17.1428571428571" customWidth="1"/>
     <col min="8" max="8" width="18.8571428571429" customWidth="1"/>
     <col min="10" max="10" width="15.8571428571429" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1346,171 +1357,207 @@
       <c r="J1" t="s">
         <v>22</v>
       </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" ht="15" spans="1:10">
+    <row r="2" ht="15" spans="1:12">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>91350</v>
       </c>
       <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" ht="15" spans="1:12">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F3" t="s">
         <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" ht="15" spans="1:10">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
       </c>
       <c r="G3">
         <v>91350</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" ht="15" spans="1:10">
+    <row r="4" ht="15" spans="1:12">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4">
         <v>91355</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="5" ht="15" spans="1:10">
+    <row r="5" ht="15" spans="1:12">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5">
         <v>91390</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:12">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" ht="15" spans="1:10">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
       </c>
       <c r="G6">
         <v>91340</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="shloka@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="Mahika@gmail.com" tooltip="mailto:Mahika@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="Nickc@gmail.com" tooltip="mailto:Nickc@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="Nickolascook@gmail.com" tooltip="mailto:Nickolascook@gmail.com"/>
     <hyperlink ref="C4" r:id="rId3" display="Shlok@gmail.com"/>
     <hyperlink ref="C5" r:id="rId4" display="PjOSE@YAHOO.COM"/>
     <hyperlink ref="C6" r:id="rId5" display="samplil@yahoo.co.in"/>

</xml_diff>